<commit_message>
Remember to Fix indexes, include dealer PO
</commit_message>
<xml_diff>
--- a/sample/User_File_Template.xlsx
+++ b/sample/User_File_Template.xlsx
@@ -3,23 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Commerce\EPIC\Support\JIRA\HDM-123\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14910" windowHeight="7575"/>
   </bookViews>
   <sheets>
     <sheet name="SAP_File_Template" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>PO</t>
   </si>
@@ -64,6 +60,9 @@
   </si>
   <si>
     <t>Expedite the shipping</t>
+  </si>
+  <si>
+    <t>ZEXtest3</t>
   </si>
 </sst>
 </file>
@@ -874,7 +873,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,7 +950,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>1326456</v>

</xml_diff>